<commit_message>
1.  Support for more loop switching (#2001)
2. Supports two Meter Selection

Co-authored-by: THAPE\tiankaihe <1204973192@qq.com>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_Motor_TypeOneCoordination_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_Motor_TypeOneCoordination_19DX101.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="电动机（分立元件）" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="221">
   <si>
     <t>断路器规格</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -778,10 +778,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>接触器规格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Installed Capacity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -863,6 +859,50 @@
   </si>
   <si>
     <t>CJ20-225/3P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导体根数x每根导体截面积1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导体根数x每根导体截面积2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导体根数x每根导体截面积1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导体根数x每根导体截面积2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接触器规格3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1208,20 +1248,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1244,7 +1284,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1307,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -1290,7 +1330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -1313,7 +1353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -1336,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1359,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -1382,7 +1422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -1405,7 +1445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1428,7 +1468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -1451,7 +1491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -1474,7 +1514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.5</v>
       </c>
@@ -1497,7 +1537,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1520,7 +1560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -1543,7 +1583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18.5</v>
       </c>
@@ -1566,7 +1606,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -1589,7 +1629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -1612,7 +1652,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37</v>
       </c>
@@ -1635,7 +1675,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -1658,7 +1698,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>55</v>
       </c>
@@ -1681,7 +1721,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -1704,7 +1744,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>90</v>
       </c>
@@ -1727,7 +1767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>110</v>
       </c>
@@ -1750,7 +1790,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>132</v>
       </c>
@@ -1773,7 +1813,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>160</v>
       </c>
@@ -1796,7 +1836,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>200</v>
       </c>
@@ -1834,15 +1874,15 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1859,7 +1899,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1876,7 +1916,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -1894,7 +1934,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -1912,7 +1952,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -1930,7 +1970,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1948,7 +1988,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -1966,7 +2006,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -1984,7 +2024,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2002,7 +2042,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2020,7 +2060,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -2038,7 +2078,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.5</v>
       </c>
@@ -2056,7 +2096,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2074,7 +2114,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -2092,7 +2132,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18.5</v>
       </c>
@@ -2110,7 +2150,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -2128,7 +2168,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -2146,7 +2186,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37</v>
       </c>
@@ -2164,7 +2204,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -2182,7 +2222,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>55</v>
       </c>
@@ -2200,7 +2240,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -2218,7 +2258,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>90</v>
       </c>
@@ -2236,7 +2276,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>110</v>
       </c>
@@ -2265,21 +2305,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2293,25 +2333,25 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2343,7 +2383,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -2375,7 +2415,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -2407,7 +2447,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -2439,7 +2479,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -2471,7 +2511,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -2503,7 +2543,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -2535,7 +2575,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2567,7 +2607,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2599,7 +2639,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -2631,7 +2671,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.5</v>
       </c>
@@ -2663,7 +2703,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2695,7 +2735,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -2727,7 +2767,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18.5</v>
       </c>
@@ -2759,7 +2799,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -2791,7 +2831,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -2823,7 +2863,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37</v>
       </c>
@@ -2855,7 +2895,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -2887,7 +2927,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>55</v>
       </c>
@@ -2919,7 +2959,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -2951,7 +2991,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>90</v>
       </c>
@@ -2983,7 +3023,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>110</v>
       </c>
@@ -3015,7 +3055,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>132</v>
       </c>
@@ -3047,7 +3087,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>160</v>
       </c>
@@ -3079,7 +3119,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>200</v>
       </c>
@@ -3111,7 +3151,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>250</v>
       </c>
@@ -3143,7 +3183,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>315</v>
       </c>
@@ -3187,19 +3227,19 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3213,19 +3253,19 @@
         <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>216</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>217</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3251,7 +3291,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -3277,7 +3317,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -3303,7 +3343,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -3329,7 +3369,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -3355,7 +3395,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -3381,7 +3421,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3407,7 +3447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -3433,7 +3473,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -3459,7 +3499,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -3485,7 +3525,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.5</v>
       </c>
@@ -3511,7 +3551,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3537,7 +3577,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -3563,7 +3603,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18.5</v>
       </c>
@@ -3589,7 +3629,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -3615,7 +3655,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -3641,7 +3681,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37</v>
       </c>
@@ -3667,7 +3707,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -3693,7 +3733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>55</v>
       </c>
@@ -3719,7 +3759,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -3745,7 +3785,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>90</v>
       </c>
@@ -3771,7 +3811,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>110</v>
       </c>
@@ -3809,17 +3849,17 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
@@ -3830,30 +3870,30 @@
         <v>188</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.37</v>
       </c>
@@ -3864,14 +3904,14 @@
         <v>4.2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.55000000000000004</v>
       </c>
@@ -3882,14 +3922,14 @@
         <v>6.8</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.75</v>
       </c>
@@ -3900,14 +3940,14 @@
         <v>12.2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -3918,14 +3958,14 @@
         <v>16.8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -3936,14 +3976,14 @@
         <v>23.3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -3954,14 +3994,14 @@
         <v>32.4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -3972,14 +4012,14 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -3990,14 +4030,14 @@
         <v>60.1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5.5</v>
       </c>
@@ -4008,14 +4048,14 @@
         <v>75.5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.5</v>
       </c>
@@ -4026,14 +4066,14 @@
         <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4044,14 +4084,14 @@
         <v>159</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -4062,14 +4102,14 @@
         <v>221</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18.5</v>
       </c>
@@ -4080,14 +4120,14 @@
         <v>293</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -4098,14 +4138,14 @@
         <v>387</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -4116,14 +4156,14 @@
         <v>382</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37</v>
       </c>
@@ -4134,14 +4174,14 @@
         <v>492</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -4152,14 +4192,14 @@
         <v>655</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>55</v>
       </c>
@@ -4170,14 +4210,14 @@
         <v>745</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -4188,14 +4228,14 @@
         <v>1107</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>90</v>
       </c>
@@ -4206,14 +4246,14 @@
         <v>1302</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>110</v>
       </c>
@@ -4224,14 +4264,14 @@
         <v>1319</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>132</v>
       </c>
@@ -4242,11 +4282,11 @@
         <v>1549</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>160</v>
       </c>
@@ -4257,11 +4297,11 @@
         <v>1960</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>200</v>
       </c>
@@ -4272,7 +4312,7 @@
         <v>2342</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H26" s="1"/>
     </row>

</xml_diff>